<commit_message>
added text and better data
</commit_message>
<xml_diff>
--- a/data/flea_dog.xlsx
+++ b/data/flea_dog.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">animal</t>
   </si>
@@ -21,6 +21,9 @@
   </si>
   <si>
     <t xml:space="preserve">flea_count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weight</t>
   </si>
   <si>
     <t xml:space="preserve">grade</t>
@@ -377,10 +380,13 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="n">
         <v>5.7</v>
@@ -389,15 +395,18 @@
         <v>18</v>
       </c>
       <c r="D2" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="E2" t="n">
         <v>8</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="n">
         <v>8.9</v>
@@ -406,15 +415,18 @@
         <v>22</v>
       </c>
       <c r="D3" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="E3" t="n">
         <v>8</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="n">
         <v>11.8</v>
@@ -423,66 +435,78 @@
         <v>17</v>
       </c>
       <c r="D4" t="n">
-        <v>6</v>
+        <v>2.8</v>
       </c>
       <c r="E4" t="n">
+        <v>6</v>
+      </c>
+      <c r="F4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>8.2</v>
+        <v>5.6</v>
       </c>
       <c r="C5" t="n">
         <v>12</v>
       </c>
       <c r="D5" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="E5" t="n">
         <v>8</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>5.6</v>
+        <v>9.1</v>
       </c>
       <c r="C6" t="n">
         <v>23</v>
       </c>
       <c r="D6" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="E6" t="n">
         <v>7</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>9.1</v>
+        <v>8.2</v>
       </c>
       <c r="C7" t="n">
         <v>18</v>
       </c>
       <c r="D7" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="E7" t="n">
         <v>7</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" t="n">
         <v>7.6</v>
@@ -491,9 +515,12 @@
         <v>21</v>
       </c>
       <c r="D8" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="E8" t="n">
         <v>9</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>